<commit_message>
Atualizado IMC.XLSX e IMC_APCS.XLSX
</commit_message>
<xml_diff>
--- a/outputs/sisaprophelper#autoaprop/autoapropxlsx/IMC_APCS.XLSX
+++ b/outputs/sisaprophelper#autoaprop/autoapropxlsx/IMC_APCS.XLSX
@@ -133,10 +133,10 @@
     <t>JOSE ANTONIO DE BARROS</t>
   </si>
   <si>
-    <t>AMARILDO ROSA PEREIRA</t>
+    <t>ALLAN NEVES DE PAULA</t>
   </si>
   <si>
-    <t>ALLAN NEVES DE PAULA</t>
+    <t> </t>
   </si>
   <si>
     <t> </t>
@@ -151,10 +151,10 @@
     <t>2459</t>
   </si>
   <si>
-    <t>2727</t>
+    <t>3552</t>
   </si>
   <si>
-    <t>3552</t>
+    <t> </t>
   </si>
   <si>
     <t> </t>
@@ -173,10 +173,10 @@
     <t>IMC_APCS</t>
   </si>
   <si>
-    <t>JOSE ANTONIO DE BARROS</t>
+    <t>ALLAN NEVES DE PAULA</t>
   </si>
   <si>
-    <t>Matr.: 2459</t>
+    <t>Matr.: 3552</t>
   </si>
   <si>
     <r>
@@ -3524,11 +3524,11 @@
       <c r="N12" s="161"/>
       <c r="O12" s="187" t="str">
         <f>H12</f>
-        <v>AMARILDO ROSA PEREIRA</v>
+        <v>ALLAN NEVES DE PAULA</v>
       </c>
       <c r="P12" s="161" t="str">
         <f>I12</f>
-        <v>ALLAN NEVES DE PAULA</v>
+        <v> </v>
       </c>
       <c r="Q12" s="161" t="str">
         <f>J12</f>
@@ -3551,11 +3551,11 @@
       <c r="W12" s="161"/>
       <c r="X12" s="161" t="str">
         <f>H12</f>
-        <v>AMARILDO ROSA PEREIRA</v>
+        <v>ALLAN NEVES DE PAULA</v>
       </c>
       <c r="Y12" s="161" t="str">
         <f>I12</f>
-        <v>ALLAN NEVES DE PAULA</v>
+        <v> </v>
       </c>
       <c r="Z12" s="161" t="str">
         <f>J12</f>
@@ -3575,11 +3575,11 @@
       </c>
       <c r="AD12" s="183" t="str">
         <f t="shared" si="0"/>
-        <v>AMARILDO ROSA PEREIRA</v>
+        <v>ALLAN NEVES DE PAULA</v>
       </c>
       <c r="AE12" s="161" t="str">
         <f t="shared" si="0"/>
-        <v>ALLAN NEVES DE PAULA</v>
+        <v> </v>
       </c>
       <c r="AF12" s="161" t="str">
         <f t="shared" si="0"/>
@@ -3599,11 +3599,11 @@
       </c>
       <c r="AJ12" s="183" t="str">
         <f t="shared" si="1"/>
-        <v>AMARILDO ROSA PEREIRA</v>
+        <v>ALLAN NEVES DE PAULA</v>
       </c>
       <c r="AK12" s="161" t="str">
         <f t="shared" si="1"/>
-        <v>ALLAN NEVES DE PAULA</v>
+        <v> </v>
       </c>
       <c r="AL12" s="161" t="str">
         <f t="shared" si="1"/>
@@ -3904,11 +3904,11 @@
       <c r="N19" s="172"/>
       <c r="O19" s="172" t="str">
         <f>H19</f>
-        <v>2727</v>
+        <v>3552</v>
       </c>
       <c r="P19" s="172" t="str">
         <f>I19</f>
-        <v>3552</v>
+        <v> </v>
       </c>
       <c r="Q19" s="172" t="str">
         <f>J19</f>
@@ -3931,11 +3931,11 @@
       <c r="W19" s="172"/>
       <c r="X19" s="172" t="str">
         <f>H19</f>
-        <v>2727</v>
+        <v>3552</v>
       </c>
       <c r="Y19" s="172" t="str">
         <f>I19</f>
-        <v>3552</v>
+        <v> </v>
       </c>
       <c r="Z19" s="172" t="str">
         <f>J19</f>
@@ -3955,11 +3955,11 @@
       </c>
       <c r="AD19" s="172" t="str">
         <f t="shared" si="2"/>
-        <v>2727</v>
+        <v>3552</v>
       </c>
       <c r="AE19" s="172" t="str">
         <f t="shared" si="2"/>
-        <v>3552</v>
+        <v> </v>
       </c>
       <c r="AF19" s="172" t="str">
         <f t="shared" si="2"/>
@@ -3979,11 +3979,11 @@
       </c>
       <c r="AJ19" s="172" t="str">
         <f t="shared" si="3"/>
-        <v>2727</v>
+        <v>3552</v>
       </c>
       <c r="AK19" s="172" t="str">
         <f t="shared" si="3"/>
-        <v>3552</v>
+        <v> </v>
       </c>
       <c r="AL19" s="172" t="str">
         <f t="shared" si="3"/>
@@ -6326,7 +6326,7 @@
       <c r="E6" s="115"/>
       <c r="F6" s="104" t="str">
         <f>'Segunda a Sexta'!F6:L6</f>
-        <v>JOSE ANTONIO DE BARROS</v>
+        <v>ALLAN NEVES DE PAULA</v>
       </c>
       <c r="G6" s="105"/>
       <c r="H6" s="105"/>
@@ -6415,7 +6415,7 @@
       <c r="E8" s="115"/>
       <c r="F8" s="104" t="str">
         <f>'Segunda a Sexta'!F8:L8</f>
-        <v>Matr.: 2459</v>
+        <v>Matr.: 3552</v>
       </c>
       <c r="G8" s="105"/>
       <c r="H8" s="105"/>
@@ -6609,11 +6609,11 @@
       </c>
       <c r="H12" s="161" t="str">
         <f>'Segunda a Sexta'!H12:H18</f>
-        <v>AMARILDO ROSA PEREIRA</v>
+        <v>ALLAN NEVES DE PAULA</v>
       </c>
       <c r="I12" s="161" t="str">
         <f>'Segunda a Sexta'!I12:I18</f>
-        <v>ALLAN NEVES DE PAULA</v>
+        <v> </v>
       </c>
       <c r="J12" s="161" t="str">
         <f>'Segunda a Sexta'!J12:J18</f>
@@ -6634,11 +6634,11 @@
       <c r="N12" s="161"/>
       <c r="O12" s="187" t="str">
         <f>'Segunda a Sexta'!H12:H18</f>
-        <v>AMARILDO ROSA PEREIRA</v>
+        <v>ALLAN NEVES DE PAULA</v>
       </c>
       <c r="P12" s="187" t="str">
         <f>'Segunda a Sexta'!I12:I18</f>
-        <v>ALLAN NEVES DE PAULA</v>
+        <v> </v>
       </c>
       <c r="Q12" s="187" t="str">
         <f>'Segunda a Sexta'!J12:J18</f>
@@ -6941,11 +6941,11 @@
       </c>
       <c r="H19" s="168" t="str">
         <f>'Segunda a Sexta'!H19:H20</f>
-        <v>2727</v>
+        <v>3552</v>
       </c>
       <c r="I19" s="168" t="str">
         <f>'Segunda a Sexta'!I19:I20</f>
-        <v>3552</v>
+        <v> </v>
       </c>
       <c r="J19" s="170" t="str">
         <f>'Segunda a Sexta'!J19:J20</f>
@@ -6966,11 +6966,11 @@
       <c r="N19" s="172"/>
       <c r="O19" s="257" t="str">
         <f>'Segunda a Sexta'!H19:H20</f>
-        <v>2727</v>
+        <v>3552</v>
       </c>
       <c r="P19" s="257" t="str">
         <f>'Segunda a Sexta'!I19:I20</f>
-        <v>3552</v>
+        <v> </v>
       </c>
       <c r="Q19" s="257" t="str">
         <f>'Segunda a Sexta'!J19:J20</f>

</xml_diff>